<commit_message>
add more PDFs and Xiamen
</commit_message>
<xml_diff>
--- a/哈尔滨/哈尔滨.xlsx
+++ b/哈尔滨/哈尔滨.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="行程" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,17 @@
     <sheet name="住宿" sheetId="3" r:id="rId3"/>
     <sheet name="景点门票" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>时间</t>
   </si>
@@ -43,9 +48,6 @@
     <t>大连-上海，南方航空CZ6535</t>
   </si>
   <si>
-    <t>哈尔滨-大连 火车T130</t>
-  </si>
-  <si>
     <t>冰雪大世界成人门票</t>
   </si>
   <si>
@@ -86,17 +88,25 @@
   </si>
   <si>
     <t>地点</t>
+  </si>
+  <si>
+    <t>次日10：13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈尔滨-上海，特快软卧</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -104,7 +114,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -133,16 +157,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -150,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -162,9 +186,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -636,9 +663,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -646,17 +673,23 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -665,17 +698,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -692,7 +725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>41675</v>
       </c>
@@ -710,64 +743,67 @@
         <v>801</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:5">
+      <c r="A3" s="7">
+        <v>41679</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
         <v>41678</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.9277777777777777</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.32013888888888892</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>41679</v>
-      </c>
       <c r="B4" s="3">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.83680555555555547</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E4" s="4">
-        <f>1982/2</f>
-        <v>991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>767.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4">
-        <f>SUM(E2:E4)</f>
-        <v>2022</v>
+        <f>SUM(E2:E5)</f>
+        <v>1568.5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -779,28 +815,28 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -809,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>41675</v>
       </c>
@@ -817,20 +853,20 @@
         <v>41677</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="4">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>41677</v>
       </c>
@@ -838,20 +874,20 @@
         <v>41678</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -860,7 +896,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -873,8 +909,14 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -886,15 +928,15 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>4</v>
@@ -903,19 +945,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2">
         <v>270</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update some schedule of haerbin
</commit_message>
<xml_diff>
--- a/哈尔滨/哈尔滨.xlsx
+++ b/哈尔滨/哈尔滨.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="行程" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="住宿" sheetId="3" r:id="rId3"/>
     <sheet name="景点门票" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>时间</t>
   </si>
@@ -112,17 +112,29 @@
   </si>
   <si>
     <t>http://item.taobao.com/item.htm?spm=2013.1.0.0.k9Z9MR&amp;id=18516323039</t>
+  </si>
+  <si>
+    <t>冰雪大世界</t>
+  </si>
+  <si>
+    <t>酒店入住</t>
+  </si>
+  <si>
+    <t>晚饭，大连市区逛逛</t>
+  </si>
+  <si>
+    <t>到达，午饭</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -130,7 +142,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -138,13 +150,13 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -152,7 +164,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,7 +172,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -179,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -202,6 +214,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -214,7 +263,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -231,17 +280,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -707,41 +768,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="12">
+        <v>41675</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="13"/>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="13"/>
+      <c r="B4" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="14"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="12">
+        <v>41676</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="13"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="14"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12">
+        <v>41677</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="13"/>
+      <c r="B10" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="14"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="12">
+        <v>41678</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="13"/>
+      <c r="B13" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="14"/>
+      <c r="B14" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="15">
+        <v>41679</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B20">
+      <c r="B18">
         <f>SUM(外部交通!E6+住宿!E6+住宿!G5+景点门票!G5+景点门票!C5)</f>
         <v>2108.5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -757,14 +967,14 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -882,15 +1092,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1017,10 +1227,10 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
update haerbin total price
</commit_message>
<xml_diff>
--- a/哈尔滨/哈尔滨.xlsx
+++ b/哈尔滨/哈尔滨.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>时间</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>到达，午饭</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -280,6 +283,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -288,9 +294,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -771,7 +774,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -797,7 +800,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="12">
+      <c r="A2" s="13">
         <v>41675</v>
       </c>
       <c r="B2" s="3">
@@ -810,7 +813,7 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="13"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3">
         <v>0.5</v>
       </c>
@@ -821,7 +824,7 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3">
         <v>0.54166666666666663</v>
       </c>
@@ -832,14 +835,14 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>41676</v>
       </c>
       <c r="B6" s="4"/>
@@ -848,21 +851,21 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <v>41677</v>
       </c>
       <c r="B9" s="3"/>
@@ -871,7 +874,7 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3">
         <v>0.625</v>
       </c>
@@ -882,14 +885,14 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>41678</v>
       </c>
       <c r="B12" s="3">
@@ -902,7 +905,7 @@
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3">
         <v>0.625</v>
       </c>
@@ -913,7 +916,7 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="14"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3">
         <v>0.66666666666666663</v>
       </c>
@@ -924,7 +927,7 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="15">
+      <c r="A15" s="12">
         <v>41679</v>
       </c>
       <c r="B15" s="3">
@@ -942,7 +945,7 @@
       </c>
       <c r="B18">
         <f>SUM(外部交通!E6+住宿!E6+住宿!G5+景点门票!G5+景点门票!C5)</f>
-        <v>2108.5</v>
+        <v>2378.5</v>
       </c>
     </row>
   </sheetData>
@@ -1221,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1252,6 +1255,15 @@
         <v>27</v>
       </c>
       <c r="C2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <f>SUM(C2:C4)</f>
         <v>270</v>
       </c>
     </row>

</xml_diff>